<commit_message>
corrected name cummulated --> cumulated
</commit_message>
<xml_diff>
--- a/data_vaccines_numbers.xlsx
+++ b/data_vaccines_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407339C1-D2E1-455E-9641-CE14138DA89E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC47CC6-CC76-4744-97F2-095F1B895931}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="12192" windowHeight="13320" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccine approval" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <author>tc={21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}</author>
   </authors>
   <commentList>
-    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -48,7 +48,7 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="G18" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+    <comment ref="G16" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -56,7 +56,7 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="G19" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
+    <comment ref="G17" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
   <si>
     <t>country</t>
   </si>
@@ -155,7 +155,7 @@
     <t>https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/</t>
   </si>
   <si>
-    <t>shipping_volume_forecast_cummulated</t>
+    <t>shipping_volume_forecast_cumulated</t>
   </si>
 </sst>
 </file>
@@ -559,13 +559,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+  <threadedComment ref="G15" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
-  <threadedComment ref="G18" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+  <threadedComment ref="G16" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
-  <threadedComment ref="G19" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
+  <threadedComment ref="G17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
 </ThreadedComments>
@@ -573,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B207B-0EB6-4EF4-88FB-421592296A82}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,7 @@
         <v>7500000</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ref="F11:F16" si="3">E11/G11</f>
+        <f t="shared" ref="F11:F14" si="3">E11/G11</f>
         <v>3750000</v>
       </c>
       <c r="G11" s="4">
@@ -1099,7 +1099,7 @@
         <v>15</v>
       </c>
       <c r="I13" s="1">
-        <v>44228</v>
+        <v>44230</v>
       </c>
       <c r="J13" s="4">
         <v>0</v>
@@ -1159,72 +1159,84 @@
         <v>12</v>
       </c>
       <c r="B15" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>44173</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4">
-        <v>7500000</v>
+        <v>5300000</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="3"/>
-        <v>3750000</v>
-      </c>
-      <c r="G15" s="4">
-        <v>2</v>
+        <f t="shared" ref="F15" si="4">E15/G15</f>
+        <v>3533333.3333333335</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1.5</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I15" s="1">
-        <v>44316</v>
+        <v>44197</v>
       </c>
       <c r="J15" s="4">
         <v>0</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>44173</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E16" s="4">
-        <v>7500000</v>
+        <v>5300000</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="3"/>
-        <v>3750000</v>
-      </c>
-      <c r="G16" s="4">
-        <v>2</v>
+        <f t="shared" ref="F16:F17" si="5">E16/G16</f>
+        <v>3533333.3333333335</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1.5</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I16" s="1">
-        <v>44316</v>
+        <v>44227</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
       </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1243,7 +1255,7 @@
         <v>5300000</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" ref="F17" si="4">E17/G17</f>
+        <f t="shared" si="5"/>
         <v>3533333.3333333335</v>
       </c>
       <c r="G17" s="5">
@@ -1253,117 +1265,33 @@
         <v>21</v>
       </c>
       <c r="I17" s="1">
-        <v>44197</v>
+        <v>44227</v>
       </c>
       <c r="J17" s="4">
         <v>0</v>
       </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1">
-        <v>44173</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="4">
-        <v>5300000</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" ref="F18:F19" si="5">E18/G18</f>
-        <v>3533333.3333333335</v>
-      </c>
-      <c r="G18" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="H18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="1">
-        <v>44227</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="1">
-        <v>44173</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="4">
-        <v>5300000</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="5"/>
-        <v>3533333.3333333335</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="1">
-        <v>44227</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="9"/>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E8567AFD-F948-4690-A799-1E8401B37C92}"/>
-    <hyperlink ref="C17" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
+    <hyperlink ref="C15" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
     <hyperlink ref="C11" r:id="rId3" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{246D7B2B-C6AC-4855-A710-0B7EB86FC31B}"/>
     <hyperlink ref="C13" r:id="rId5" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{65B1E0B5-520F-417B-A93C-D2870E54C409}"/>
-    <hyperlink ref="C18" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
-    <hyperlink ref="C19" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
+    <hyperlink ref="C16" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
+    <hyperlink ref="C17" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
     <hyperlink ref="C14" r:id="rId8" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{1A41E538-3658-4ECB-A121-4CB5B41913A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1382,12 +1310,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DED90A92496A7744ABCE13896B9F92DA" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b49787f72d67ac0aa2c3a374ebf068f2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d5bda608be47ebbf9612181af6292e1" ns2:_="">
     <xsd:import namespace="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
@@ -1537,6 +1459,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C96820-C391-4B7C-A57F-E7A178B5A878}">
   <ds:schemaRefs>
@@ -1546,22 +1474,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2D919F7-6F5F-4E1C-ABD8-8F275E6A7768}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9893CF25-92F4-48D2-9BBB-695FEE2AB90C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1577,4 +1489,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2D919F7-6F5F-4E1C-ABD8-8F275E6A7768}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated impf_daten (BAG 5.2.) and vaccines number
</commit_message>
<xml_diff>
--- a/data_vaccines_numbers.xlsx
+++ b/data_vaccines_numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D013770E-5013-455C-9844-321B95FFE212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5855CCA5-8E47-4ECE-AC18-8A5DCC597DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <author>tc={21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}</author>
   </authors>
   <commentList>
-    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -48,7 +48,7 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="G16" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+    <comment ref="G17" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -56,7 +56,7 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="G17" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
+    <comment ref="G18" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>country</t>
   </si>
@@ -559,13 +559,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G15" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+  <threadedComment ref="G16" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
-  <threadedComment ref="G16" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+  <threadedComment ref="G17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
-  <threadedComment ref="G17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
+  <threadedComment ref="G18" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
 </ThreadedComments>
@@ -573,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B207B-0EB6-4EF4-88FB-421592296A82}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -842,10 +842,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>44228</v>
+        <v>44232</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -854,7 +854,7 @@
         <v>3000000</v>
       </c>
       <c r="F7" s="4">
-        <f>E7/G7</f>
+        <f t="shared" ref="F7" si="2">E7/G7</f>
         <v>1500000</v>
       </c>
       <c r="G7" s="4">
@@ -864,19 +864,13 @@
         <v>15</v>
       </c>
       <c r="I7" s="1">
-        <v>44228</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4">
-        <v>22217</v>
-      </c>
-      <c r="M7" s="4">
-        <f>SUM(L$7:L7)+K$6</f>
-        <v>354077</v>
-      </c>
-      <c r="N7" t="s">
-        <v>18</v>
-      </c>
+        <v>44230</v>
+      </c>
+      <c r="K7" s="4">
+        <v>337800</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -905,15 +899,18 @@
         <v>15</v>
       </c>
       <c r="I8" s="1">
-        <v>44235</v>
+        <v>44228</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4">
-        <v>18729</v>
+        <v>22217</v>
       </c>
       <c r="M8" s="4">
-        <f>SUM(L$7:L8)+K$6</f>
-        <v>372806</v>
+        <f>SUM(L$8:L8)+K$6</f>
+        <v>354077</v>
+      </c>
+      <c r="N8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -943,15 +940,15 @@
         <v>15</v>
       </c>
       <c r="I9" s="1">
-        <v>44242</v>
+        <v>44235</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4">
-        <v>170000</v>
+        <v>18729</v>
       </c>
       <c r="M9" s="4">
-        <f>SUM(L$7:L9)+K$6</f>
-        <v>542806</v>
+        <f>SUM(L$8:L9)+K$6</f>
+        <v>372806</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -959,18 +956,20 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>44208</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>44228</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>3000000</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" ref="F10" si="2">E10/G10</f>
-        <v>0</v>
+        <f>E10/G10</f>
+        <v>1500000</v>
       </c>
       <c r="G10" s="4">
         <v>2</v>
@@ -979,37 +978,34 @@
         <v>15</v>
       </c>
       <c r="I10" s="1">
-        <v>44197</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <f>SUM(J10:J$10)</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+        <v>44242</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
+        <v>170000</v>
+      </c>
+      <c r="M10" s="4">
+        <f>SUM(L$8:L10)+K$6</f>
+        <v>542806</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>44209</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>24</v>
-      </c>
+        <v>44208</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="4">
-        <v>7500000</v>
+        <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ref="F11:F14" si="3">E11/G11</f>
-        <v>3750000</v>
+        <f t="shared" ref="F11" si="3">E11/G11</f>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
@@ -1018,30 +1014,27 @@
         <v>15</v>
       </c>
       <c r="I11" s="1">
-        <v>44209</v>
+        <v>44197</v>
       </c>
       <c r="J11" s="4">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4">
-        <f>SUM(J$10:J11)</f>
-        <v>200000</v>
+        <f>SUM(J11:J$11)</f>
+        <v>0</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>44209</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -1050,7 +1043,7 @@
         <v>7500000</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F12:F15" si="4">E12/G12</f>
         <v>3750000</v>
       </c>
       <c r="G12" s="4">
@@ -1060,27 +1053,30 @@
         <v>15</v>
       </c>
       <c r="I12" s="1">
-        <v>44227</v>
+        <v>44209</v>
       </c>
       <c r="J12" s="4">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="K12" s="4">
-        <f>SUM(J$10:J12)</f>
+        <f>SUM(J$11:J12)</f>
         <v>200000</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>44228</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>27</v>
+        <v>44188</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -1089,7 +1085,7 @@
         <v>7500000</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3750000</v>
       </c>
       <c r="G13" s="4">
@@ -1099,26 +1095,24 @@
         <v>15</v>
       </c>
       <c r="I13" s="1">
-        <v>44228</v>
+        <v>44227</v>
       </c>
       <c r="J13" s="4">
         <v>0</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4">
-        <v>300000</v>
-      </c>
-      <c r="M13" s="4">
-        <f>SUM(L$13:L13)+K$12</f>
-        <v>500000</v>
-      </c>
+      <c r="K13" s="4">
+        <f>SUM(J$11:J13)</f>
+        <v>200000</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>44188</v>
+        <v>44228</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>27</v>
@@ -1130,7 +1124,7 @@
         <v>7500000</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3750000</v>
       </c>
       <c r="G14" s="4">
@@ -1140,18 +1134,18 @@
         <v>15</v>
       </c>
       <c r="I14" s="1">
-        <v>44249</v>
+        <v>44228</v>
       </c>
       <c r="J14" s="4">
         <v>0</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4">
-        <v>400000</v>
+        <v>300000</v>
       </c>
       <c r="M14" s="4">
-        <f>SUM(L$13:L14)+K$12</f>
-        <v>900000</v>
+        <f>SUM(L$14:L14)+K$13</f>
+        <v>500000</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1159,41 +1153,40 @@
         <v>12</v>
       </c>
       <c r="B15" s="1">
-        <v>44173</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>22</v>
+        <v>44188</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4">
-        <v>5300000</v>
+        <v>7500000</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" ref="F15" si="4">E15/G15</f>
-        <v>3533333.3333333335</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1.5</v>
+        <f t="shared" si="4"/>
+        <v>3750000</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I15" s="1">
-        <v>44197</v>
+        <v>44249</v>
       </c>
       <c r="J15" s="4">
         <v>0</v>
       </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
+      <c r="K15" s="4"/>
       <c r="L15" s="4">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="M15" s="4">
-        <v>0</v>
+        <f>SUM(L$14:L15)+K$13</f>
+        <v>900000</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1213,7 +1206,7 @@
         <v>5300000</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16:F17" si="5">E16/G16</f>
+        <f t="shared" ref="F16" si="5">E16/G16</f>
         <v>3533333.3333333335</v>
       </c>
       <c r="G16" s="5">
@@ -1223,7 +1216,7 @@
         <v>21</v>
       </c>
       <c r="I16" s="1">
-        <v>44227</v>
+        <v>44197</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
@@ -1255,7 +1248,7 @@
         <v>5300000</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F17:F18" si="6">E17/G17</f>
         <v>3533333.3333333335</v>
       </c>
       <c r="G17" s="5">
@@ -1270,30 +1263,72 @@
       <c r="J17" s="4">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="9"/>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44173</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4">
+        <v>5300000</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="6"/>
+        <v>3533333.3333333335</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="1">
+        <v>44227</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E8567AFD-F948-4690-A799-1E8401B37C92}"/>
-    <hyperlink ref="C15" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
-    <hyperlink ref="C11" r:id="rId3" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
+    <hyperlink ref="C16" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
+    <hyperlink ref="C12" r:id="rId3" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{246D7B2B-C6AC-4855-A710-0B7EB86FC31B}"/>
-    <hyperlink ref="C13" r:id="rId5" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{65B1E0B5-520F-417B-A93C-D2870E54C409}"/>
-    <hyperlink ref="C16" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
-    <hyperlink ref="C17" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
-    <hyperlink ref="C14" r:id="rId8" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{1A41E538-3658-4ECB-A121-4CB5B41913A5}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{1E860BC1-31E0-4921-A3E7-D0ECDCEE39A2}"/>
+    <hyperlink ref="C14" r:id="rId5" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{65B1E0B5-520F-417B-A93C-D2870E54C409}"/>
+    <hyperlink ref="C17" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
+    <hyperlink ref="C18" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
+    <hyperlink ref="C15" r:id="rId8" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{1A41E538-3658-4ECB-A121-4CB5B41913A5}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{1E860BC1-31E0-4921-A3E7-D0ECDCEE39A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId10"/>
@@ -1302,12 +1337,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1461,15 +1493,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C96820-C391-4B7C-A57F-E7A178B5A878}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2D919F7-6F5F-4E1C-ABD8-8F275E6A7768}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1493,17 +1536,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2D919F7-6F5F-4E1C-ABD8-8F275E6A7768}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C96820-C391-4B7C-A57F-E7A178B5A878}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
pfizer up to 6M
</commit_message>
<xml_diff>
--- a/data_vaccines_numbers.xlsx
+++ b/data_vaccines_numbers.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5855CCA5-8E47-4ECE-AC18-8A5DCC597DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{5855CCA5-8E47-4ECE-AC18-8A5DCC597DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{06C61FA7-3D2B-4CD7-AE86-B8CDA034E961}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccine approval" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'vaccine approval'!$A$1:$N$26</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +43,7 @@
     <author>tc={21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}</author>
   </authors>
   <commentList>
-    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -48,7 +51,7 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="G17" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+    <comment ref="G18" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -56,7 +59,7 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="G18" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
+    <comment ref="G19" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -69,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>country</t>
   </si>
@@ -156,6 +159,9 @@
   </si>
   <si>
     <t>shipping_volume_forecast_cumulated</t>
+  </si>
+  <si>
+    <t>nzz 27.3.21</t>
   </si>
 </sst>
 </file>
@@ -559,13 +565,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G16" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+  <threadedComment ref="G17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
-  <threadedComment ref="G17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+  <threadedComment ref="G18" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
-  <threadedComment ref="G18" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
+  <threadedComment ref="G19" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
 </ThreadedComments>
@@ -573,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B207B-0EB6-4EF4-88FB-421592296A82}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -650,7 +656,7 @@
         <v>3000000</v>
       </c>
       <c r="F2" s="4">
-        <f>E2/G2</f>
+        <f t="shared" ref="F2:F19" si="0">E2/G2</f>
         <v>1500000</v>
       </c>
       <c r="G2" s="4">
@@ -692,7 +698,7 @@
         <v>3000000</v>
       </c>
       <c r="F3" s="4">
-        <f>E3/G3</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G3" s="4">
@@ -734,7 +740,7 @@
         <v>3000000</v>
       </c>
       <c r="F4" s="4">
-        <f>E4/G4</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G4" s="4">
@@ -776,7 +782,7 @@
         <v>3000000</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5" si="0">E5/G5</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G5" s="4">
@@ -815,7 +821,7 @@
         <v>3000000</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6" si="1">E6/G6</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G6" s="4">
@@ -854,7 +860,7 @@
         <v>3000000</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ref="F7" si="2">E7/G7</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G7" s="4">
@@ -889,7 +895,7 @@
         <v>3000000</v>
       </c>
       <c r="F8" s="4">
-        <f>E8/G8</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G8" s="4">
@@ -930,7 +936,7 @@
         <v>3000000</v>
       </c>
       <c r="F9" s="4">
-        <f>E9/G9</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G9" s="4">
@@ -968,7 +974,7 @@
         <v>3000000</v>
       </c>
       <c r="F10" s="4">
-        <f>E10/G10</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="G10" s="4">
@@ -994,18 +1000,20 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>44208</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>44282</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E11" s="4">
-        <v>0</v>
+        <v>6000000</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ref="F11" si="3">E11/G11</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3000000</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
@@ -1013,16 +1021,8 @@
       <c r="H11" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="1">
-        <v>44197</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <f>SUM(J11:J$11)</f>
-        <v>0</v>
-      </c>
+      <c r="I11" s="1"/>
+      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
@@ -1031,20 +1031,18 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>44209</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>24</v>
-      </c>
+        <v>44208</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="4">
-        <v>7500000</v>
+        <v>0</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" ref="F12:F15" si="4">E12/G12</f>
-        <v>3750000</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
         <v>2</v>
@@ -1053,30 +1051,27 @@
         <v>15</v>
       </c>
       <c r="I12" s="1">
-        <v>44209</v>
+        <v>44197</v>
       </c>
       <c r="J12" s="4">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="K12" s="4">
-        <f>SUM(J$11:J12)</f>
-        <v>200000</v>
+        <f>SUM(J12:J$12)</f>
+        <v>0</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>44209</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -1085,7 +1080,7 @@
         <v>7500000</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>3750000</v>
       </c>
       <c r="G13" s="4">
@@ -1095,27 +1090,30 @@
         <v>15</v>
       </c>
       <c r="I13" s="1">
-        <v>44227</v>
+        <v>44209</v>
       </c>
       <c r="J13" s="4">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="K13" s="4">
-        <f>SUM(J$11:J13)</f>
+        <f>SUM(J$7:J17)</f>
         <v>200000</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
+      <c r="N13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>44228</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>27</v>
+        <v>44188</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -1124,7 +1122,7 @@
         <v>7500000</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>3750000</v>
       </c>
       <c r="G14" s="4">
@@ -1134,26 +1132,24 @@
         <v>15</v>
       </c>
       <c r="I14" s="1">
-        <v>44228</v>
+        <v>44227</v>
       </c>
       <c r="J14" s="4">
         <v>0</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4">
-        <v>300000</v>
-      </c>
-      <c r="M14" s="4">
-        <f>SUM(L$14:L14)+K$13</f>
-        <v>500000</v>
-      </c>
+      <c r="K14" s="4">
+        <f>SUM(J$10:J15)</f>
+        <v>200000</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1">
-        <v>44188</v>
+        <v>44228</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>27</v>
@@ -1165,7 +1161,7 @@
         <v>7500000</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>3750000</v>
       </c>
       <c r="G15" s="4">
@@ -1175,18 +1171,18 @@
         <v>15</v>
       </c>
       <c r="I15" s="1">
-        <v>44249</v>
+        <v>44228</v>
       </c>
       <c r="J15" s="4">
         <v>0</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4">
-        <v>400000</v>
+        <v>300000</v>
       </c>
       <c r="M15" s="4">
-        <f>SUM(L$14:L15)+K$13</f>
-        <v>900000</v>
+        <f>SUM(L$15:L15)+K$14</f>
+        <v>500000</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1194,41 +1190,40 @@
         <v>12</v>
       </c>
       <c r="B16" s="1">
-        <v>44173</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>22</v>
+        <v>44188</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16" s="4">
-        <v>5300000</v>
+        <v>7500000</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16" si="5">E16/G16</f>
-        <v>3533333.3333333335</v>
-      </c>
-      <c r="G16" s="5">
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>3750000</v>
+      </c>
+      <c r="G16" s="4">
+        <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I16" s="1">
-        <v>44197</v>
+        <v>44249</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
       </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="M16" s="4">
-        <v>0</v>
+        <f>SUM(L$15:L16)+K$14</f>
+        <v>900000</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1248,7 +1243,7 @@
         <v>5300000</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" ref="F17:F18" si="6">E17/G17</f>
+        <f t="shared" si="0"/>
         <v>3533333.3333333335</v>
       </c>
       <c r="G17" s="5">
@@ -1258,7 +1253,7 @@
         <v>21</v>
       </c>
       <c r="I17" s="1">
-        <v>44227</v>
+        <v>44197</v>
       </c>
       <c r="J17" s="4">
         <v>0</v>
@@ -1290,7 +1285,7 @@
         <v>5300000</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>3533333.3333333335</v>
       </c>
       <c r="G18" s="5">
@@ -1305,34 +1300,140 @@
       <c r="J18" s="4">
         <v>0</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C25" s="9"/>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44173</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5300000</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>3533333.3333333335</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="1">
+        <v>44227</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C26" s="9"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I28" s="1">
+        <v>44185</v>
+      </c>
+      <c r="J28" s="4">
+        <v>107000</v>
+      </c>
+      <c r="K28">
+        <v>107000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I29" s="1">
+        <v>44200</v>
+      </c>
+      <c r="J29" s="4">
+        <v>126000</v>
+      </c>
+      <c r="K29">
+        <v>233000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I30" s="1">
+        <v>44209</v>
+      </c>
+      <c r="J30" s="4">
+        <v>200000</v>
+      </c>
+      <c r="K30">
+        <f>K29+200000</f>
+        <v>433000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I31" s="1">
+        <v>44220</v>
+      </c>
+      <c r="J31" s="4">
+        <v>38400</v>
+      </c>
+      <c r="K31">
+        <f>271400+200000</f>
+        <v>471400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N26" xr:uid="{7716E730-1812-44CC-B733-AB46996EFF44}"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E8567AFD-F948-4690-A799-1E8401B37C92}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
-    <hyperlink ref="C12" r:id="rId3" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
+    <hyperlink ref="C13" r:id="rId3" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{246D7B2B-C6AC-4855-A710-0B7EB86FC31B}"/>
-    <hyperlink ref="C14" r:id="rId5" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{65B1E0B5-520F-417B-A93C-D2870E54C409}"/>
-    <hyperlink ref="C17" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
-    <hyperlink ref="C18" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
-    <hyperlink ref="C15" r:id="rId8" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{1A41E538-3658-4ECB-A121-4CB5B41913A5}"/>
+    <hyperlink ref="C15" r:id="rId5" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{65B1E0B5-520F-417B-A93C-D2870E54C409}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
+    <hyperlink ref="C16" r:id="rId8" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{1A41E538-3658-4ECB-A121-4CB5B41913A5}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{1E860BC1-31E0-4921-A3E7-D0ECDCEE39A2}"/>
+    <hyperlink ref="C11" r:id="rId10" display="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{8AC72EBF-2A4F-4797-86A8-0A8E9B7D247D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>